<commit_message>
improve my code to new files, improve excel retriving and add Average
</commit_message>
<xml_diff>
--- a/DataBase/costs.xlsx
+++ b/DataBase/costs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="18975" windowHeight="11760"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2108" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2112" uniqueCount="521">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1574,17 +1574,20 @@
   </si>
   <si>
     <t>ταξί από Άγ.Αντώνιο με Νίκο</t>
+  </si>
+  <si>
+    <t>αεροπορικά για Ιρλανδία</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1625,9 +1628,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
     <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
@@ -1692,6 +1695,9 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1706,10 +1712,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A1:H530" totalsRowShown="0">
-  <autoFilter ref="A1:H530"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:H530" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="8">
-    <tableColumn id="1" name="amount" totalsRowDxfId="7"/>
+    <tableColumn id="1" name="amount" headerRowDxfId="8" totalsRowDxfId="7"/>
     <tableColumn id="11" name="type" totalsRowDxfId="6"/>
     <tableColumn id="2" name="date" totalsRowDxfId="5"/>
     <tableColumn id="4" name="description" totalsRowDxfId="4"/>
@@ -1718,12 +1723,12 @@
     <tableColumn id="7" name="weather" totalsRowDxfId="1"/>
     <tableColumn id="8" name="location" totalsRowDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Θέμα του Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1765,7 +1770,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1797,9 +1802,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1831,6 +1837,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2006,14 +2013,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L528"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A505" workbookViewId="0">
-      <selection activeCell="D526" sqref="D526"/>
+    <sheetView tabSelected="1" topLeftCell="A467" workbookViewId="0">
+      <selection activeCell="B482" sqref="B482"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
@@ -2029,8 +2036,8 @@
     <col min="12" max="12" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>234</v>
       </c>
       <c r="B1" t="s">
@@ -2058,7 +2065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>488</v>
       </c>
@@ -2084,7 +2091,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>20</v>
       </c>
@@ -2108,7 +2115,7 @@
       </c>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>10</v>
       </c>
@@ -2131,7 +2138,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>100</v>
       </c>
@@ -2154,7 +2161,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>10</v>
       </c>
@@ -2177,7 +2184,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>50</v>
       </c>
@@ -2200,7 +2207,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>3.2</v>
       </c>
@@ -2223,7 +2230,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>1.3</v>
       </c>
@@ -2246,7 +2253,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>1.2</v>
       </c>
@@ -2269,7 +2276,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>5</v>
       </c>
@@ -2292,7 +2299,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>4.5</v>
       </c>
@@ -2315,7 +2322,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>4</v>
       </c>
@@ -2338,7 +2345,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>10.6</v>
       </c>
@@ -2361,7 +2368,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>1.8</v>
       </c>
@@ -2384,7 +2391,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>5.15</v>
       </c>
@@ -2407,7 +2414,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>18</v>
       </c>
@@ -2430,7 +2437,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>1.5</v>
       </c>
@@ -2453,7 +2460,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>7.8</v>
       </c>
@@ -2476,7 +2483,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>4.4400000000000004</v>
       </c>
@@ -2499,7 +2506,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>1.5</v>
       </c>
@@ -2522,7 +2529,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>8.84</v>
       </c>
@@ -2545,7 +2552,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>4</v>
       </c>
@@ -2568,7 +2575,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>10</v>
       </c>
@@ -2591,7 +2598,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>1.8</v>
       </c>
@@ -2614,7 +2621,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>11.8</v>
       </c>
@@ -2637,7 +2644,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>40</v>
       </c>
@@ -2660,7 +2667,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>2.9</v>
       </c>
@@ -2683,7 +2690,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>4.3</v>
       </c>
@@ -2706,7 +2713,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>3.35</v>
       </c>
@@ -2729,7 +2736,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>5.2</v>
       </c>
@@ -2752,7 +2759,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>15</v>
       </c>
@@ -2775,7 +2782,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>3.9</v>
       </c>
@@ -2798,7 +2805,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>63.45</v>
       </c>
@@ -2821,7 +2828,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>49.9</v>
       </c>
@@ -2841,7 +2848,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>140</v>
       </c>
@@ -2864,7 +2871,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>1.8</v>
       </c>
@@ -2887,7 +2894,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>13.02</v>
       </c>
@@ -2910,7 +2917,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>4.7</v>
       </c>
@@ -2933,7 +2940,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>15.96</v>
       </c>
@@ -2956,7 +2963,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>9.8000000000000007</v>
       </c>
@@ -2979,7 +2986,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>79.8</v>
       </c>
@@ -3002,7 +3009,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>11.9</v>
       </c>
@@ -3025,7 +3032,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>38.880000000000003</v>
       </c>
@@ -3048,7 +3055,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>7.75</v>
       </c>
@@ -3071,7 +3078,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>0.79</v>
       </c>
@@ -3094,7 +3101,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>10</v>
       </c>
@@ -3117,7 +3124,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -3140,7 +3147,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -3163,7 +3170,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>1.8</v>
       </c>
@@ -3186,7 +3193,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>24</v>
       </c>
@@ -3209,7 +3216,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>24</v>
       </c>
@@ -3232,7 +3239,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>1.8</v>
       </c>
@@ -3255,7 +3262,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>3.5</v>
       </c>
@@ -3278,7 +3285,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>5.6</v>
       </c>
@@ -3302,7 +3309,7 @@
       </c>
       <c r="K55" s="4"/>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>1.5</v>
       </c>
@@ -3325,7 +3332,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>3</v>
       </c>
@@ -3348,7 +3355,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>5.4</v>
       </c>
@@ -3371,7 +3378,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>8</v>
       </c>
@@ -3394,7 +3401,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>5.4</v>
       </c>
@@ -3417,7 +3424,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>0.6</v>
       </c>
@@ -3440,7 +3447,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -3463,7 +3470,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>1.5</v>
       </c>
@@ -3486,7 +3493,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -3509,7 +3516,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>1.2</v>
       </c>
@@ -3532,7 +3539,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>5.0999999999999996</v>
       </c>
@@ -3555,7 +3562,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>13.5</v>
       </c>
@@ -3578,7 +3585,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>3.5</v>
       </c>
@@ -3602,7 +3609,7 @@
       </c>
       <c r="K68" s="4"/>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>4.0999999999999996</v>
       </c>
@@ -3625,7 +3632,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>90</v>
       </c>
@@ -3648,7 +3655,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>65.5</v>
       </c>
@@ -3671,7 +3678,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>4.5</v>
       </c>
@@ -3694,7 +3701,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>10</v>
       </c>
@@ -3717,7 +3724,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>18.8</v>
       </c>
@@ -3740,7 +3747,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>1.8</v>
       </c>
@@ -3764,7 +3771,7 @@
       </c>
       <c r="K75" s="4"/>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>5.5</v>
       </c>
@@ -3787,7 +3794,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -3810,7 +3817,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>3</v>
       </c>
@@ -3833,7 +3840,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>2</v>
       </c>
@@ -3856,7 +3863,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>9.9</v>
       </c>
@@ -3879,7 +3886,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>6.5</v>
       </c>
@@ -3902,7 +3909,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>79.8</v>
       </c>
@@ -3925,7 +3932,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>10</v>
       </c>
@@ -3948,7 +3955,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>2.5</v>
       </c>
@@ -3971,7 +3978,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <v>5</v>
       </c>
@@ -3994,7 +4001,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>1.6</v>
       </c>
@@ -4017,7 +4024,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <v>5.5</v>
       </c>
@@ -4040,7 +4047,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
         <v>0.8</v>
       </c>
@@ -4063,7 +4070,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <v>17</v>
       </c>
@@ -4086,7 +4093,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <v>24.9</v>
       </c>
@@ -4109,7 +4116,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
         <v>1.8</v>
       </c>
@@ -4132,7 +4139,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <v>44.99</v>
       </c>
@@ -4155,7 +4162,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <v>4</v>
       </c>
@@ -4178,7 +4185,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <v>5</v>
       </c>
@@ -4201,7 +4208,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <v>5</v>
       </c>
@@ -4224,7 +4231,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -4247,7 +4254,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
         <v>3</v>
       </c>
@@ -4270,7 +4277,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <v>6</v>
       </c>
@@ -4293,7 +4300,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <v>3.5</v>
       </c>
@@ -4316,7 +4323,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <v>34.9</v>
       </c>
@@ -4339,7 +4346,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <v>12</v>
       </c>
@@ -4362,7 +4369,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <v>5</v>
       </c>
@@ -4385,7 +4392,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
         <v>6.9</v>
       </c>
@@ -4408,7 +4415,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
         <v>6.04</v>
       </c>
@@ -4431,7 +4438,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="4">
         <v>4.8</v>
       </c>
@@ -4454,7 +4461,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="4">
         <v>9.6999999999999993</v>
       </c>
@@ -4477,7 +4484,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
         <v>5.5</v>
       </c>
@@ -4500,7 +4507,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="4">
         <v>7</v>
       </c>
@@ -4523,7 +4530,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="4">
         <v>1</v>
       </c>
@@ -4546,7 +4553,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="4">
         <v>4</v>
       </c>
@@ -4569,7 +4576,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="4">
         <v>4.0999999999999996</v>
       </c>
@@ -4592,7 +4599,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="112" spans="1:8">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="4">
         <v>2.3199999999999998</v>
       </c>
@@ -4615,7 +4622,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="4">
         <v>8</v>
       </c>
@@ -4638,7 +4645,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="4">
         <v>12.5</v>
       </c>
@@ -4661,7 +4668,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="4">
         <v>0.7</v>
       </c>
@@ -4684,7 +4691,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="4">
         <v>6.3</v>
       </c>
@@ -4707,7 +4714,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="4">
         <v>8</v>
       </c>
@@ -4730,7 +4737,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="4">
         <v>5.0999999999999996</v>
       </c>
@@ -4753,7 +4760,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="4">
         <v>8</v>
       </c>
@@ -4776,7 +4783,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="4">
         <v>4.5</v>
       </c>
@@ -4799,7 +4806,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="4">
         <v>2.5</v>
       </c>
@@ -4822,7 +4829,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="4">
         <v>24.3</v>
       </c>
@@ -4845,7 +4852,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="4">
         <v>2</v>
       </c>
@@ -4868,7 +4875,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="4">
         <v>16</v>
       </c>
@@ -4891,7 +4898,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="4">
         <v>6</v>
       </c>
@@ -4914,7 +4921,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="126" spans="1:8">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="4">
         <v>5</v>
       </c>
@@ -4937,7 +4944,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="127" spans="1:8">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="4">
         <v>6.52</v>
       </c>
@@ -4960,7 +4967,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="128" spans="1:8">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="4">
         <v>1.8</v>
       </c>
@@ -4983,7 +4990,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="129" spans="1:8">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="4">
         <v>1</v>
       </c>
@@ -5006,7 +5013,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="130" spans="1:8">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="4">
         <v>5</v>
       </c>
@@ -5029,7 +5036,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="131" spans="1:8">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="4">
         <v>43</v>
       </c>
@@ -5052,7 +5059,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="132" spans="1:8">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="4">
         <v>10</v>
       </c>
@@ -5075,7 +5082,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="133" spans="1:8">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="4">
         <v>2.97</v>
       </c>
@@ -5098,7 +5105,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="134" spans="1:8">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="4">
         <v>10</v>
       </c>
@@ -5121,7 +5128,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="135" spans="1:8">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="4">
         <v>1.6</v>
       </c>
@@ -5144,7 +5151,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="136" spans="1:8">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="4">
         <v>1.5</v>
       </c>
@@ -5167,7 +5174,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="137" spans="1:8">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="4">
         <v>1.8</v>
       </c>
@@ -5190,7 +5197,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="138" spans="1:8">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="4">
         <v>7.3</v>
       </c>
@@ -5213,7 +5220,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="139" spans="1:8">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="4">
         <v>4</v>
       </c>
@@ -5236,7 +5243,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="140" spans="1:8">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="4">
         <v>2.1</v>
       </c>
@@ -5259,7 +5266,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="141" spans="1:8">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="4">
         <v>4.2</v>
       </c>
@@ -5282,7 +5289,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="142" spans="1:8">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="4">
         <v>9</v>
       </c>
@@ -5305,7 +5312,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="143" spans="1:8">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="4">
         <v>1</v>
       </c>
@@ -5328,7 +5335,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="144" spans="1:8">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="4">
         <v>3.5</v>
       </c>
@@ -5351,7 +5358,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="145" spans="1:8">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="4">
         <v>5.0999999999999996</v>
       </c>
@@ -5374,7 +5381,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="146" spans="1:8">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="4">
         <v>3</v>
       </c>
@@ -5397,7 +5404,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="147" spans="1:8">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="4">
         <v>2</v>
       </c>
@@ -5420,7 +5427,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="148" spans="1:8">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="4">
         <v>150</v>
       </c>
@@ -5443,7 +5450,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="149" spans="1:8">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="4">
         <v>7</v>
       </c>
@@ -5466,7 +5473,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="150" spans="1:8">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="4">
         <v>5</v>
       </c>
@@ -5489,7 +5496,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="151" spans="1:8">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="4">
         <v>8</v>
       </c>
@@ -5512,7 +5519,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="152" spans="1:8">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="4">
         <v>3.5</v>
       </c>
@@ -5535,7 +5542,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="153" spans="1:8">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="4">
         <v>55</v>
       </c>
@@ -5558,7 +5565,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="154" spans="1:8">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="4">
         <v>0.6</v>
       </c>
@@ -5581,7 +5588,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="155" spans="1:8">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="4">
         <v>4</v>
       </c>
@@ -5604,7 +5611,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="156" spans="1:8">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="4">
         <v>39.9</v>
       </c>
@@ -5627,7 +5634,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="157" spans="1:8">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="4">
         <v>1.6</v>
       </c>
@@ -5650,7 +5657,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="158" spans="1:8">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="4">
         <v>80</v>
       </c>
@@ -5673,7 +5680,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="159" spans="1:8">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="4">
         <v>6.2</v>
       </c>
@@ -5696,7 +5703,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="160" spans="1:8">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="4">
         <v>15</v>
       </c>
@@ -5719,7 +5726,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="161" spans="1:8">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="4">
         <v>4.3</v>
       </c>
@@ -5742,7 +5749,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="162" spans="1:8">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="4">
         <v>9.6999999999999993</v>
       </c>
@@ -5765,7 +5772,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="163" spans="1:8">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="4">
         <v>2.4500000000000002</v>
       </c>
@@ -5788,7 +5795,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="164" spans="1:8">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="4">
         <v>1.96</v>
       </c>
@@ -5811,7 +5818,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="165" spans="1:8">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="4">
         <v>11.5</v>
       </c>
@@ -5834,7 +5841,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="166" spans="1:8">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="4">
         <v>2.7</v>
       </c>
@@ -5857,7 +5864,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="167" spans="1:8">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="4">
         <v>2.7</v>
       </c>
@@ -5880,7 +5887,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="168" spans="1:8">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="4">
         <v>7</v>
       </c>
@@ -5903,7 +5910,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="169" spans="1:8">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="4">
         <v>4.8</v>
       </c>
@@ -5926,7 +5933,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="170" spans="1:8">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="4">
         <v>4.4000000000000004</v>
       </c>
@@ -5949,7 +5956,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="171" spans="1:8">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="4">
         <v>3.8</v>
       </c>
@@ -5972,7 +5979,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="172" spans="1:8">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="4">
         <v>1.5</v>
       </c>
@@ -5995,7 +6002,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="173" spans="1:8">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="4">
         <v>11.5</v>
       </c>
@@ -6018,7 +6025,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="174" spans="1:8">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="4">
         <v>4.4000000000000004</v>
       </c>
@@ -6041,7 +6048,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="175" spans="1:8">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="4">
         <v>6.5</v>
       </c>
@@ -6064,7 +6071,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="176" spans="1:8">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="4">
         <v>6.5</v>
       </c>
@@ -6087,7 +6094,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="177" spans="1:8">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="4">
         <v>5</v>
       </c>
@@ -6110,7 +6117,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="178" spans="1:8">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="4">
         <v>6</v>
       </c>
@@ -6133,7 +6140,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="179" spans="1:8">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="4">
         <v>8</v>
       </c>
@@ -6156,7 +6163,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="180" spans="1:8">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="4">
         <v>3.2</v>
       </c>
@@ -6179,7 +6186,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="181" spans="1:8">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="4">
         <v>10</v>
       </c>
@@ -6202,7 +6209,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="182" spans="1:8">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="4">
         <v>3</v>
       </c>
@@ -6225,7 +6232,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="183" spans="1:8">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="4">
         <v>10</v>
       </c>
@@ -6248,7 +6255,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="184" spans="1:8">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="4">
         <v>3.5</v>
       </c>
@@ -6271,7 +6278,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="185" spans="1:8">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="4">
         <v>10</v>
       </c>
@@ -6294,7 +6301,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="186" spans="1:8">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="4">
         <v>8</v>
       </c>
@@ -6317,7 +6324,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="187" spans="1:8">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" s="4">
         <v>6.2</v>
       </c>
@@ -6340,7 +6347,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="188" spans="1:8">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" s="4">
         <v>2</v>
       </c>
@@ -6363,7 +6370,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="189" spans="1:8">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" s="4">
         <v>10</v>
       </c>
@@ -6386,7 +6393,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="190" spans="1:8">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" s="4">
         <v>22</v>
       </c>
@@ -6409,7 +6416,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="191" spans="1:8">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" s="4">
         <v>14</v>
       </c>
@@ -6432,7 +6439,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="192" spans="1:8">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" s="4">
         <v>14</v>
       </c>
@@ -6455,7 +6462,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="193" spans="1:8">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" s="4">
         <v>4.7</v>
       </c>
@@ -6478,7 +6485,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="194" spans="1:8">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" s="4">
         <v>69.900000000000006</v>
       </c>
@@ -6501,7 +6508,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="195" spans="1:8">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" s="4">
         <v>8.4</v>
       </c>
@@ -6524,7 +6531,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="196" spans="1:8">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" s="4">
         <v>5</v>
       </c>
@@ -6547,7 +6554,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="197" spans="1:8">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" s="4">
         <v>4.5</v>
       </c>
@@ -6570,7 +6577,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="198" spans="1:8">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198" s="4">
         <v>6</v>
       </c>
@@ -6593,7 +6600,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="199" spans="1:8">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" s="4">
         <v>5.46</v>
       </c>
@@ -6616,7 +6623,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="200" spans="1:8">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" s="4">
         <v>78.849999999999994</v>
       </c>
@@ -6639,7 +6646,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="201" spans="1:8">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" s="4">
         <v>10</v>
       </c>
@@ -6662,7 +6669,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="202" spans="1:8">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" s="4">
         <v>10</v>
       </c>
@@ -6685,7 +6692,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="203" spans="1:8">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" s="4">
         <v>26</v>
       </c>
@@ -6708,7 +6715,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="204" spans="1:8">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204" s="4">
         <v>2</v>
       </c>
@@ -6731,7 +6738,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="205" spans="1:8">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205" s="4">
         <v>2.5</v>
       </c>
@@ -6754,7 +6761,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="206" spans="1:8">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" s="4">
         <v>5.9</v>
       </c>
@@ -6777,7 +6784,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="207" spans="1:8">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" s="4">
         <v>8.6</v>
       </c>
@@ -6800,7 +6807,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="208" spans="1:8">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208" s="4">
         <v>2.7</v>
       </c>
@@ -6823,7 +6830,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="209" spans="1:8">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209" s="4">
         <v>4.8</v>
       </c>
@@ -6846,7 +6853,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="210" spans="1:8">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210" s="4">
         <v>2.8</v>
       </c>
@@ -6869,7 +6876,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="211" spans="1:8">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211" s="4">
         <v>2</v>
       </c>
@@ -6892,7 +6899,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="212" spans="1:8">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212" s="4">
         <v>5</v>
       </c>
@@ -6915,7 +6922,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="213" spans="1:8">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213" s="4">
         <v>2.5</v>
       </c>
@@ -6938,7 +6945,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="214" spans="1:8">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214" s="4">
         <v>3.5</v>
       </c>
@@ -6961,7 +6968,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="215" spans="1:8">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" s="4">
         <v>1.8</v>
       </c>
@@ -6984,7 +6991,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="216" spans="1:8">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216" s="4">
         <v>4</v>
       </c>
@@ -7007,7 +7014,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="217" spans="1:8">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A217" s="4">
         <v>6</v>
       </c>
@@ -7030,7 +7037,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="218" spans="1:8">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218" s="4">
         <v>1.8</v>
       </c>
@@ -7053,7 +7060,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="219" spans="1:8">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219" s="4">
         <v>5</v>
       </c>
@@ -7076,7 +7083,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="220" spans="1:8">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" s="4">
         <v>5</v>
       </c>
@@ -7099,7 +7106,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="221" spans="1:8">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221" s="4">
         <v>4.7</v>
       </c>
@@ -7122,7 +7129,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="222" spans="1:8">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222" s="4">
         <v>5</v>
       </c>
@@ -7145,7 +7152,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="223" spans="1:8">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223" s="4">
         <v>10</v>
       </c>
@@ -7168,7 +7175,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="224" spans="1:8">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224" s="4">
         <v>1.5</v>
       </c>
@@ -7191,7 +7198,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="225" spans="1:8">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A225" s="4">
         <v>129</v>
       </c>
@@ -7214,7 +7221,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="226" spans="1:8">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A226" s="4">
         <v>7</v>
       </c>
@@ -7237,7 +7244,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="227" spans="1:8">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A227" s="4">
         <v>2.8</v>
       </c>
@@ -7260,7 +7267,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="228" spans="1:8">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A228" s="4">
         <v>1</v>
       </c>
@@ -7283,7 +7290,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="229" spans="1:8">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A229" s="4">
         <v>4</v>
       </c>
@@ -7306,7 +7313,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="230" spans="1:8">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A230" s="4">
         <v>50</v>
       </c>
@@ -7329,7 +7336,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="231" spans="1:8">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A231" s="4">
         <v>7.2</v>
       </c>
@@ -7352,7 +7359,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="232" spans="1:8">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A232" s="4">
         <v>1</v>
       </c>
@@ -7375,7 +7382,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="233" spans="1:8">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A233" s="4">
         <v>7</v>
       </c>
@@ -7398,7 +7405,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="234" spans="1:8">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A234" s="4">
         <v>1.1000000000000001</v>
       </c>
@@ -7421,7 +7428,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="235" spans="1:8">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A235" s="4">
         <v>7</v>
       </c>
@@ -7444,7 +7451,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="236" spans="1:8">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A236" s="4">
         <v>15</v>
       </c>
@@ -7467,7 +7474,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="237" spans="1:8">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A237" s="4">
         <v>3</v>
       </c>
@@ -7490,7 +7497,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="238" spans="1:8">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A238" s="4">
         <v>11.2</v>
       </c>
@@ -7513,7 +7520,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="239" spans="1:8">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A239" s="4">
         <v>2.1</v>
       </c>
@@ -7536,7 +7543,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="240" spans="1:8">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A240" s="4">
         <v>150</v>
       </c>
@@ -7559,7 +7566,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="241" spans="1:8">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A241" s="4">
         <v>12.7</v>
       </c>
@@ -7582,7 +7589,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="242" spans="1:8">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A242" s="4">
         <v>89.9</v>
       </c>
@@ -7605,7 +7612,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="243" spans="1:8">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A243" s="4">
         <v>4.4000000000000004</v>
       </c>
@@ -7628,7 +7635,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="244" spans="1:8">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A244" s="4">
         <v>4.2</v>
       </c>
@@ -7651,7 +7658,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="245" spans="1:8">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A245" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -7674,7 +7681,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="246" spans="1:8">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A246" s="4">
         <v>5</v>
       </c>
@@ -7697,7 +7704,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="247" spans="1:8">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A247" s="4">
         <v>5</v>
       </c>
@@ -7720,7 +7727,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="248" spans="1:8">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A248" s="4">
         <v>3.9</v>
       </c>
@@ -7743,7 +7750,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="249" spans="1:8">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A249" s="4">
         <v>0.5</v>
       </c>
@@ -7766,7 +7773,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="250" spans="1:8">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A250" s="4">
         <v>2.4</v>
       </c>
@@ -7789,7 +7796,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="251" spans="1:8">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A251" s="4">
         <v>2</v>
       </c>
@@ -7812,7 +7819,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="252" spans="1:8">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A252" s="4">
         <v>4.7</v>
       </c>
@@ -7835,7 +7842,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="253" spans="1:8">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A253" s="4">
         <v>5.3</v>
       </c>
@@ -7858,7 +7865,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="254" spans="1:8">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A254" s="4">
         <v>4.2</v>
       </c>
@@ -7881,7 +7888,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="255" spans="1:8">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A255" s="4">
         <v>5</v>
       </c>
@@ -7904,7 +7911,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="256" spans="1:8">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A256" s="4">
         <v>2.5</v>
       </c>
@@ -7927,7 +7934,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="257" spans="1:8">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A257" s="4">
         <v>3.3</v>
       </c>
@@ -7950,7 +7957,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="258" spans="1:8">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A258" s="4">
         <v>5.6</v>
       </c>
@@ -7973,7 +7980,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="259" spans="1:8">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A259" s="4">
         <v>4</v>
       </c>
@@ -7996,7 +8003,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="260" spans="1:8">
+    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A260" s="4">
         <v>10.199999999999999</v>
       </c>
@@ -8019,7 +8026,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="261" spans="1:8">
+    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A261" s="4">
         <v>8</v>
       </c>
@@ -8042,7 +8049,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="262" spans="1:8">
+    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A262" s="4">
         <v>2.1</v>
       </c>
@@ -8065,7 +8072,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="263" spans="1:8">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A263" s="4">
         <v>3.7</v>
       </c>
@@ -8088,7 +8095,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="264" spans="1:8">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A264" s="4">
         <v>7</v>
       </c>
@@ -8111,7 +8118,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="265" spans="1:8">
+    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A265" s="4">
         <v>13.5</v>
       </c>
@@ -8134,7 +8141,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="266" spans="1:8">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A266" s="4">
         <v>5</v>
       </c>
@@ -8157,7 +8164,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="267" spans="1:8">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A267" s="4">
         <v>20</v>
       </c>
@@ -8180,7 +8187,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="268" spans="1:8">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A268" s="4">
         <v>6</v>
       </c>
@@ -8203,7 +8210,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="269" spans="1:8">
+    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A269" s="4">
         <v>0.5</v>
       </c>
@@ -8226,7 +8233,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="270" spans="1:8">
+    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A270" s="4">
         <v>5</v>
       </c>
@@ -8249,7 +8256,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="271" spans="1:8">
+    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A271" s="4">
         <v>11</v>
       </c>
@@ -8272,7 +8279,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="272" spans="1:8">
+    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A272" s="4">
         <v>8.8000000000000007</v>
       </c>
@@ -8295,7 +8302,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="273" spans="1:8">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A273" s="4">
         <v>0.5</v>
       </c>
@@ -8318,7 +8325,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="274" spans="1:8">
+    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A274" s="4">
         <v>5</v>
       </c>
@@ -8341,7 +8348,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="275" spans="1:8">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A275" s="4">
         <v>10</v>
       </c>
@@ -8364,7 +8371,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="276" spans="1:8">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276" s="4">
         <v>15</v>
       </c>
@@ -8387,7 +8394,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="277" spans="1:8">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A277" s="4">
         <v>10</v>
       </c>
@@ -8410,7 +8417,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="278" spans="1:8">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A278" s="4">
         <v>11.9</v>
       </c>
@@ -8433,7 +8440,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="279" spans="1:8">
+    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A279" s="4">
         <v>7</v>
       </c>
@@ -8456,7 +8463,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="280" spans="1:8">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A280" s="4">
         <v>5.0999999999999996</v>
       </c>
@@ -8479,7 +8486,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="281" spans="1:8">
+    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>1.9</v>
       </c>
@@ -8502,7 +8509,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="282" spans="1:8">
+    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>119.9</v>
       </c>
@@ -8525,7 +8532,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="283" spans="1:8">
+    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>6.3</v>
       </c>
@@ -8548,7 +8555,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="284" spans="1:8">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>3.5</v>
       </c>
@@ -8571,7 +8578,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="285" spans="1:8">
+    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>1.5</v>
       </c>
@@ -8594,7 +8601,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="286" spans="1:8">
+    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>1.9</v>
       </c>
@@ -8617,7 +8624,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="287" spans="1:8">
+    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>4.5</v>
       </c>
@@ -8640,7 +8647,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="288" spans="1:8">
+    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>6.4</v>
       </c>
@@ -8663,7 +8670,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="289" spans="1:8">
+    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>1.9</v>
       </c>
@@ -8686,7 +8693,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="290" spans="1:8">
+    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>10.6</v>
       </c>
@@ -8709,7 +8716,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="291" spans="1:8">
+    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>4.5</v>
       </c>
@@ -8732,7 +8739,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="292" spans="1:8">
+    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>22.2</v>
       </c>
@@ -8755,7 +8762,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="293" spans="1:8">
+    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A293" s="6">
         <v>25</v>
       </c>
@@ -8778,7 +8785,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="294" spans="1:8">
+    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A294" s="6">
         <v>3.5</v>
       </c>
@@ -8801,7 +8808,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="295" spans="1:8">
+    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>4</v>
       </c>
@@ -8824,7 +8831,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="296" spans="1:8">
+    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>2.2000000000000002</v>
       </c>
@@ -8847,7 +8854,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="297" spans="1:8">
+    <row r="297" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>11.5</v>
       </c>
@@ -8870,7 +8877,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="298" spans="1:8">
+    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>6.3</v>
       </c>
@@ -8893,7 +8900,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="299" spans="1:8">
+    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>3.6</v>
       </c>
@@ -8916,7 +8923,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="300" spans="1:8">
+    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>15</v>
       </c>
@@ -8939,7 +8946,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="301" spans="1:8">
+    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>2</v>
       </c>
@@ -8962,7 +8969,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="302" spans="1:8">
+    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>4.5</v>
       </c>
@@ -8985,7 +8992,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="303" spans="1:8">
+    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>2.9</v>
       </c>
@@ -9008,7 +9015,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="304" spans="1:8">
+    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>3.9</v>
       </c>
@@ -9031,7 +9038,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="305" spans="1:8">
+    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>1.7</v>
       </c>
@@ -9054,7 +9061,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="306" spans="1:8">
+    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>10</v>
       </c>
@@ -9077,7 +9084,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="307" spans="1:8">
+    <row r="307" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>7.5</v>
       </c>
@@ -9100,7 +9107,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="308" spans="1:8">
+    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>10.050000000000001</v>
       </c>
@@ -9123,7 +9130,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="309" spans="1:8">
+    <row r="309" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>5</v>
       </c>
@@ -9146,7 +9153,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="310" spans="1:8">
+    <row r="310" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>3</v>
       </c>
@@ -9169,7 +9176,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="311" spans="1:8">
+    <row r="311" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>2</v>
       </c>
@@ -9192,7 +9199,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="312" spans="1:8">
+    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>10.6</v>
       </c>
@@ -9215,7 +9222,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="313" spans="1:8">
+    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>4</v>
       </c>
@@ -9238,7 +9245,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="314" spans="1:8">
+    <row r="314" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>2</v>
       </c>
@@ -9261,7 +9268,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="315" spans="1:8">
+    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>5.8</v>
       </c>
@@ -9284,7 +9291,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="316" spans="1:8">
+    <row r="316" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>5</v>
       </c>
@@ -9307,7 +9314,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="317" spans="1:8">
+    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>6.55</v>
       </c>
@@ -9330,7 +9337,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="318" spans="1:8">
+    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>2.8</v>
       </c>
@@ -9353,7 +9360,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="319" spans="1:8">
+    <row r="319" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>3.8</v>
       </c>
@@ -9376,7 +9383,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="320" spans="1:8">
+    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>9</v>
       </c>
@@ -9399,7 +9406,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="321" spans="1:8">
+    <row r="321" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>8</v>
       </c>
@@ -9422,7 +9429,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="322" spans="1:8">
+    <row r="322" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>1.5</v>
       </c>
@@ -9445,7 +9452,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="323" spans="1:8">
+    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>5</v>
       </c>
@@ -9468,7 +9475,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="324" spans="1:8">
+    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>4.5999999999999996</v>
       </c>
@@ -9491,7 +9498,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="325" spans="1:8">
+    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>0.5</v>
       </c>
@@ -9514,7 +9521,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="326" spans="1:8">
+    <row r="326" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>2.95</v>
       </c>
@@ -9537,7 +9544,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="327" spans="1:8">
+    <row r="327" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>3.8</v>
       </c>
@@ -9560,7 +9567,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="328" spans="1:8">
+    <row r="328" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>10</v>
       </c>
@@ -9583,7 +9590,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="329" spans="1:8">
+    <row r="329" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>3.85</v>
       </c>
@@ -9606,7 +9613,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="330" spans="1:8">
+    <row r="330" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>1.2</v>
       </c>
@@ -9629,7 +9636,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="331" spans="1:8">
+    <row r="331" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>2</v>
       </c>
@@ -9652,7 +9659,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="332" spans="1:8">
+    <row r="332" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>8.5</v>
       </c>
@@ -9675,7 +9682,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="333" spans="1:8">
+    <row r="333" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>4.9000000000000004</v>
       </c>
@@ -9698,7 +9705,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="334" spans="1:8">
+    <row r="334" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>10</v>
       </c>
@@ -9721,7 +9728,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="335" spans="1:8">
+    <row r="335" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>1.5</v>
       </c>
@@ -9741,7 +9748,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="336" spans="1:8">
+    <row r="336" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>350</v>
       </c>
@@ -9764,7 +9771,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="337" spans="1:8">
+    <row r="337" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>4.4000000000000004</v>
       </c>
@@ -9787,7 +9794,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="338" spans="1:8">
+    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>3.2</v>
       </c>
@@ -9810,7 +9817,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="339" spans="1:8">
+    <row r="339" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>3.8</v>
       </c>
@@ -9833,7 +9840,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="340" spans="1:8">
+    <row r="340" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>0.9</v>
       </c>
@@ -9856,7 +9863,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="341" spans="1:8">
+    <row r="341" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>6</v>
       </c>
@@ -9879,7 +9886,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="342" spans="1:8">
+    <row r="342" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>3.8</v>
       </c>
@@ -9902,7 +9909,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="343" spans="1:8">
+    <row r="343" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>2</v>
       </c>
@@ -9925,7 +9932,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="344" spans="1:8">
+    <row r="344" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>5.5</v>
       </c>
@@ -9948,7 +9955,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="345" spans="1:8">
+    <row r="345" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>43.22</v>
       </c>
@@ -9971,7 +9978,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="346" spans="1:8">
+    <row r="346" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>2</v>
       </c>
@@ -9994,7 +10001,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="347" spans="1:8">
+    <row r="347" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>7</v>
       </c>
@@ -10017,7 +10024,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="348" spans="1:8">
+    <row r="348" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>1.61</v>
       </c>
@@ -10040,7 +10047,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="349" spans="1:8">
+    <row r="349" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>20</v>
       </c>
@@ -10063,7 +10070,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="350" spans="1:8">
+    <row r="350" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>14.84</v>
       </c>
@@ -10086,7 +10093,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="351" spans="1:8">
+    <row r="351" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>5.6</v>
       </c>
@@ -10109,7 +10116,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="352" spans="1:8">
+    <row r="352" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A352">
         <v>6.8</v>
       </c>
@@ -10132,7 +10139,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="353" spans="1:12">
+    <row r="353" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A353">
         <v>7.7</v>
       </c>
@@ -10155,7 +10162,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="354" spans="1:12">
+    <row r="354" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A354">
         <v>29.4</v>
       </c>
@@ -10178,7 +10185,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="355" spans="1:12">
+    <row r="355" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A355">
         <v>0.5</v>
       </c>
@@ -10201,7 +10208,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="356" spans="1:12">
+    <row r="356" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A356">
         <v>2.2000000000000002</v>
       </c>
@@ -10224,7 +10231,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="357" spans="1:12">
+    <row r="357" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A357">
         <v>3.5</v>
       </c>
@@ -10247,7 +10254,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="358" spans="1:12">
+    <row r="358" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A358">
         <v>4.4000000000000004</v>
       </c>
@@ -10270,7 +10277,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="359" spans="1:12">
+    <row r="359" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A359">
         <v>5.7</v>
       </c>
@@ -10293,7 +10300,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="360" spans="1:12">
+    <row r="360" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A360">
         <v>7.74</v>
       </c>
@@ -10316,7 +10323,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="361" spans="1:12">
+    <row r="361" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A361">
         <v>7</v>
       </c>
@@ -10339,7 +10346,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="362" spans="1:12">
+    <row r="362" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A362">
         <v>3.8</v>
       </c>
@@ -10362,7 +10369,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="363" spans="1:12">
+    <row r="363" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A363">
         <v>100</v>
       </c>
@@ -10385,7 +10392,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="364" spans="1:12">
+    <row r="364" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A364" s="1">
         <v>5</v>
       </c>
@@ -10409,7 +10416,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="365" spans="1:12">
+    <row r="365" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A365" s="6">
         <v>2</v>
       </c>
@@ -10436,7 +10443,7 @@
       <c r="K365" s="1"/>
       <c r="L365" s="1"/>
     </row>
-    <row r="366" spans="1:12">
+    <row r="366" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A366">
         <v>7</v>
       </c>
@@ -10459,7 +10466,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="367" spans="1:12">
+    <row r="367" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A367">
         <v>50</v>
       </c>
@@ -10482,7 +10489,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="368" spans="1:12">
+    <row r="368" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A368">
         <v>10</v>
       </c>
@@ -10505,7 +10512,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="369" spans="1:8">
+    <row r="369" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A369">
         <v>10.8</v>
       </c>
@@ -10528,7 +10535,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="370" spans="1:8">
+    <row r="370" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A370">
         <v>10.5</v>
       </c>
@@ -10551,7 +10558,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="371" spans="1:8">
+    <row r="371" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A371">
         <v>5.5</v>
       </c>
@@ -10574,7 +10581,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="372" spans="1:8">
+    <row r="372" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A372">
         <v>5</v>
       </c>
@@ -10597,7 +10604,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="373" spans="1:8">
+    <row r="373" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A373">
         <v>0.5</v>
       </c>
@@ -10620,7 +10627,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="374" spans="1:8">
+    <row r="374" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A374">
         <v>10.5</v>
       </c>
@@ -10643,7 +10650,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="375" spans="1:8">
+    <row r="375" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A375">
         <v>14</v>
       </c>
@@ -10666,7 +10673,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="376" spans="1:8">
+    <row r="376" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A376">
         <v>2</v>
       </c>
@@ -10689,7 +10696,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="377" spans="1:8">
+    <row r="377" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A377">
         <v>3.5</v>
       </c>
@@ -10712,7 +10719,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="378" spans="1:8">
+    <row r="378" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A378">
         <v>3.5</v>
       </c>
@@ -10735,7 +10742,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="379" spans="1:8">
+    <row r="379" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A379">
         <v>3.5</v>
       </c>
@@ -10758,7 +10765,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="380" spans="1:8">
+    <row r="380" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A380">
         <v>2</v>
       </c>
@@ -10781,7 +10788,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="381" spans="1:8">
+    <row r="381" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A381">
         <v>2</v>
       </c>
@@ -10804,7 +10811,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="382" spans="1:8">
+    <row r="382" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A382">
         <v>2.5</v>
       </c>
@@ -10827,7 +10834,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="383" spans="1:8">
+    <row r="383" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A383">
         <v>6.5</v>
       </c>
@@ -10850,7 +10857,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="384" spans="1:8">
+    <row r="384" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A384">
         <v>3.78</v>
       </c>
@@ -10873,7 +10880,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="385" spans="1:8">
+    <row r="385" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A385">
         <v>7</v>
       </c>
@@ -10896,7 +10903,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="386" spans="1:8">
+    <row r="386" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A386">
         <v>2.5</v>
       </c>
@@ -10919,7 +10926,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="387" spans="1:8">
+    <row r="387" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A387">
         <v>2</v>
       </c>
@@ -10942,7 +10949,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="388" spans="1:8">
+    <row r="388" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A388">
         <v>1</v>
       </c>
@@ -10965,7 +10972,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="389" spans="1:8">
+    <row r="389" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A389">
         <v>10.5</v>
       </c>
@@ -10988,7 +10995,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="390" spans="1:8">
+    <row r="390" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A390">
         <v>1.5</v>
       </c>
@@ -11011,7 +11018,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="391" spans="1:8">
+    <row r="391" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A391">
         <v>2.7</v>
       </c>
@@ -11034,7 +11041,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="392" spans="1:8">
+    <row r="392" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A392">
         <v>2</v>
       </c>
@@ -11057,7 +11064,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="393" spans="1:8">
+    <row r="393" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A393">
         <v>17.5</v>
       </c>
@@ -11080,7 +11087,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="394" spans="1:8">
+    <row r="394" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A394">
         <v>43</v>
       </c>
@@ -11103,7 +11110,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="395" spans="1:8">
+    <row r="395" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A395">
         <v>69.900000000000006</v>
       </c>
@@ -11126,7 +11133,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="396" spans="1:8">
+    <row r="396" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A396">
         <v>16</v>
       </c>
@@ -11149,7 +11156,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="397" spans="1:8">
+    <row r="397" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A397">
         <v>2.2000000000000002</v>
       </c>
@@ -11172,7 +11179,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="398" spans="1:8">
+    <row r="398" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A398">
         <v>1.72</v>
       </c>
@@ -11195,7 +11202,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="399" spans="1:8">
+    <row r="399" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A399">
         <v>6</v>
       </c>
@@ -11218,7 +11225,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="400" spans="1:8">
+    <row r="400" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A400">
         <v>1.8</v>
       </c>
@@ -11241,7 +11248,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="401" spans="1:8">
+    <row r="401" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A401">
         <v>4.5999999999999996</v>
       </c>
@@ -11264,7 +11271,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="402" spans="1:8">
+    <row r="402" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A402">
         <v>27</v>
       </c>
@@ -11287,7 +11294,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="403" spans="1:8">
+    <row r="403" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A403">
         <v>14</v>
       </c>
@@ -11310,7 +11317,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="404" spans="1:8">
+    <row r="404" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A404">
         <v>2.5</v>
       </c>
@@ -11333,7 +11340,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="405" spans="1:8">
+    <row r="405" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A405">
         <v>10</v>
       </c>
@@ -11356,7 +11363,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="406" spans="1:8">
+    <row r="406" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A406">
         <v>11</v>
       </c>
@@ -11379,7 +11386,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="407" spans="1:8">
+    <row r="407" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A407">
         <v>5.55</v>
       </c>
@@ -11402,7 +11409,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="408" spans="1:8">
+    <row r="408" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A408">
         <v>3</v>
       </c>
@@ -11425,7 +11432,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="409" spans="1:8">
+    <row r="409" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A409">
         <v>3.5</v>
       </c>
@@ -11448,7 +11455,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="410" spans="1:8">
+    <row r="410" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A410">
         <v>3.8</v>
       </c>
@@ -11471,7 +11478,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="411" spans="1:8">
+    <row r="411" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A411">
         <v>4</v>
       </c>
@@ -11494,7 +11501,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="412" spans="1:8">
+    <row r="412" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A412">
         <v>8</v>
       </c>
@@ -11517,7 +11524,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="413" spans="1:8">
+    <row r="413" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A413">
         <v>11.6</v>
       </c>
@@ -11540,7 +11547,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="414" spans="1:8">
+    <row r="414" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A414">
         <v>1.6</v>
       </c>
@@ -11563,7 +11570,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="415" spans="1:8">
+    <row r="415" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A415">
         <v>44.41</v>
       </c>
@@ -11586,7 +11593,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="416" spans="1:8">
+    <row r="416" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A416">
         <v>4.8</v>
       </c>
@@ -11609,7 +11616,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="417" spans="1:8">
+    <row r="417" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A417">
         <v>1.7</v>
       </c>
@@ -11632,7 +11639,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="418" spans="1:8">
+    <row r="418" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A418">
         <v>2.85</v>
       </c>
@@ -11655,7 +11662,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="419" spans="1:8">
+    <row r="419" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A419">
         <v>6.4</v>
       </c>
@@ -11678,7 +11685,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="420" spans="1:8">
+    <row r="420" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A420">
         <v>3.5</v>
       </c>
@@ -11701,7 +11708,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="421" spans="1:8">
+    <row r="421" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A421">
         <v>6.5</v>
       </c>
@@ -11724,7 +11731,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="422" spans="1:8">
+    <row r="422" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A422">
         <v>1.2</v>
       </c>
@@ -11747,7 +11754,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="423" spans="1:8">
+    <row r="423" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A423">
         <v>4.5999999999999996</v>
       </c>
@@ -11770,7 +11777,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="424" spans="1:8">
+    <row r="424" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A424">
         <v>8</v>
       </c>
@@ -11793,7 +11800,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="425" spans="1:8">
+    <row r="425" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A425">
         <v>3.5</v>
       </c>
@@ -11816,7 +11823,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="426" spans="1:8">
+    <row r="426" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A426" s="1">
         <v>50</v>
       </c>
@@ -11840,7 +11847,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="427" spans="1:8">
+    <row r="427" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A427">
         <v>10</v>
       </c>
@@ -11863,7 +11870,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="428" spans="1:8">
+    <row r="428" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A428">
         <v>2.9</v>
       </c>
@@ -11886,7 +11893,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="429" spans="1:8">
+    <row r="429" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A429">
         <v>15</v>
       </c>
@@ -11909,7 +11916,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="430" spans="1:8">
+    <row r="430" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A430">
         <v>3.5</v>
       </c>
@@ -11932,7 +11939,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="431" spans="1:8">
+    <row r="431" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A431">
         <v>9.25</v>
       </c>
@@ -11955,7 +11962,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="432" spans="1:8">
+    <row r="432" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A432">
         <v>8</v>
       </c>
@@ -11978,7 +11985,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="433" spans="1:8">
+    <row r="433" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A433">
         <v>4.0999999999999996</v>
       </c>
@@ -12001,7 +12008,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="434" spans="1:8">
+    <row r="434" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A434">
         <v>4.9000000000000004</v>
       </c>
@@ -12024,7 +12031,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="435" spans="1:8">
+    <row r="435" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A435">
         <v>2.8</v>
       </c>
@@ -12047,7 +12054,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="436" spans="1:8">
+    <row r="436" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A436">
         <v>18.7</v>
       </c>
@@ -12070,7 +12077,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="437" spans="1:8">
+    <row r="437" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A437">
         <v>20</v>
       </c>
@@ -12093,7 +12100,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="438" spans="1:8">
+    <row r="438" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A438" s="1">
         <v>150</v>
       </c>
@@ -12117,7 +12124,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="439" spans="1:8">
+    <row r="439" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A439" s="1">
         <v>10</v>
       </c>
@@ -12141,7 +12148,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="440" spans="1:8">
+    <row r="440" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A440">
         <v>2.1</v>
       </c>
@@ -12164,7 +12171,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="441" spans="1:8">
+    <row r="441" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A441">
         <v>5</v>
       </c>
@@ -12187,7 +12194,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="442" spans="1:8">
+    <row r="442" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A442">
         <v>10</v>
       </c>
@@ -12210,7 +12217,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="443" spans="1:8">
+    <row r="443" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A443">
         <v>59</v>
       </c>
@@ -12233,7 +12240,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="444" spans="1:8">
+    <row r="444" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A444">
         <v>4</v>
       </c>
@@ -12256,7 +12263,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="445" spans="1:8">
+    <row r="445" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A445">
         <v>4.17</v>
       </c>
@@ -12279,7 +12286,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="446" spans="1:8">
+    <row r="446" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A446">
         <v>4.2</v>
       </c>
@@ -12302,7 +12309,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="447" spans="1:8">
+    <row r="447" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A447">
         <v>4.4000000000000004</v>
       </c>
@@ -12325,7 +12332,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="448" spans="1:8">
+    <row r="448" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A448">
         <v>30</v>
       </c>
@@ -12348,7 +12355,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="449" spans="1:8">
+    <row r="449" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A449">
         <v>5</v>
       </c>
@@ -12371,7 +12378,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="450" spans="1:8">
+    <row r="450" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A450">
         <v>15.7</v>
       </c>
@@ -12394,7 +12401,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="451" spans="1:8">
+    <row r="451" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A451">
         <v>4</v>
       </c>
@@ -12417,7 +12424,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="452" spans="1:8">
+    <row r="452" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A452">
         <v>8</v>
       </c>
@@ -12440,7 +12447,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="453" spans="1:8">
+    <row r="453" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A453">
         <v>3.5</v>
       </c>
@@ -12463,7 +12470,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="454" spans="1:8">
+    <row r="454" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A454">
         <v>4.2</v>
       </c>
@@ -12486,7 +12493,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="455" spans="1:8">
+    <row r="455" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A455">
         <v>180</v>
       </c>
@@ -12509,7 +12516,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="456" spans="1:8">
+    <row r="456" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A456">
         <v>2.2999999999999998</v>
       </c>
@@ -12532,7 +12539,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="457" spans="1:8">
+    <row r="457" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A457">
         <v>11</v>
       </c>
@@ -12555,7 +12562,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="458" spans="1:8">
+    <row r="458" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A458">
         <v>2</v>
       </c>
@@ -12578,7 +12585,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="459" spans="1:8">
+    <row r="459" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A459">
         <v>3</v>
       </c>
@@ -12601,7 +12608,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="460" spans="1:8">
+    <row r="460" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A460">
         <v>6.4</v>
       </c>
@@ -12624,7 +12631,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="461" spans="1:8">
+    <row r="461" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A461">
         <v>3.2</v>
       </c>
@@ -12647,7 +12654,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="462" spans="1:8">
+    <row r="462" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A462">
         <v>1</v>
       </c>
@@ -12670,7 +12677,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="463" spans="1:8">
+    <row r="463" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A463">
         <v>4.2</v>
       </c>
@@ -12693,7 +12700,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="464" spans="1:8">
+    <row r="464" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A464">
         <v>14</v>
       </c>
@@ -12716,7 +12723,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="465" spans="1:8">
+    <row r="465" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A465">
         <v>2.9</v>
       </c>
@@ -12739,7 +12746,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="466" spans="1:8">
+    <row r="466" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A466">
         <v>4</v>
       </c>
@@ -12762,7 +12769,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="467" spans="1:8">
+    <row r="467" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A467">
         <v>1.8</v>
       </c>
@@ -12785,7 +12792,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="468" spans="1:8">
+    <row r="468" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A468">
         <v>18</v>
       </c>
@@ -12808,7 +12815,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="469" spans="1:8">
+    <row r="469" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A469">
         <v>2</v>
       </c>
@@ -12831,7 +12838,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="470" spans="1:8">
+    <row r="470" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A470">
         <v>3</v>
       </c>
@@ -12854,7 +12861,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="471" spans="1:8">
+    <row r="471" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A471">
         <v>10</v>
       </c>
@@ -12877,7 +12884,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="472" spans="1:8">
+    <row r="472" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A472">
         <v>8.3000000000000007</v>
       </c>
@@ -12900,12 +12907,12 @@
         <v>241</v>
       </c>
     </row>
-    <row r="473" spans="1:8">
+    <row r="473" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A473">
         <v>362</v>
       </c>
       <c r="B473" t="s">
-        <v>344</v>
+        <v>352</v>
       </c>
       <c r="C473" s="2">
         <v>43374</v>
@@ -12923,7 +12930,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="474" spans="1:8">
+    <row r="474" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A474">
         <v>4.2</v>
       </c>
@@ -12946,7 +12953,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="475" spans="1:8">
+    <row r="475" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A475">
         <v>0.5</v>
       </c>
@@ -12969,7 +12976,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="476" spans="1:8">
+    <row r="476" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A476">
         <v>1.7</v>
       </c>
@@ -12992,7 +12999,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="477" spans="1:8">
+    <row r="477" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A477">
         <v>4.5999999999999996</v>
       </c>
@@ -13015,7 +13022,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="478" spans="1:8">
+    <row r="478" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A478">
         <v>4.7</v>
       </c>
@@ -13038,7 +13045,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="479" spans="1:8">
+    <row r="479" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A479">
         <v>1</v>
       </c>
@@ -13061,7 +13068,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="480" spans="1:8">
+    <row r="480" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A480">
         <v>5.6</v>
       </c>
@@ -13084,12 +13091,12 @@
         <v>250</v>
       </c>
     </row>
-    <row r="481" spans="1:8">
+    <row r="481" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A481">
         <v>33.799999999999997</v>
       </c>
       <c r="B481" t="s">
-        <v>344</v>
+        <v>352</v>
       </c>
       <c r="C481" s="2">
         <v>43377</v>
@@ -13107,7 +13114,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="482" spans="1:8">
+    <row r="482" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A482">
         <v>8</v>
       </c>
@@ -13130,7 +13137,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="483" spans="1:8">
+    <row r="483" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A483">
         <v>5.2</v>
       </c>
@@ -13153,7 +13160,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="484" spans="1:8">
+    <row r="484" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A484">
         <v>5.4</v>
       </c>
@@ -13176,7 +13183,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="485" spans="1:8">
+    <row r="485" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A485">
         <v>40</v>
       </c>
@@ -13199,7 +13206,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="486" spans="1:8">
+    <row r="486" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A486">
         <v>10.8</v>
       </c>
@@ -13222,7 +13229,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="487" spans="1:8">
+    <row r="487" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A487">
         <v>15</v>
       </c>
@@ -13245,7 +13252,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="488" spans="1:8">
+    <row r="488" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A488">
         <v>20</v>
       </c>
@@ -13268,7 +13275,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="489" spans="1:8">
+    <row r="489" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A489">
         <v>3</v>
       </c>
@@ -13291,7 +13298,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="490" spans="1:8">
+    <row r="490" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A490">
         <v>3.5</v>
       </c>
@@ -13314,7 +13321,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="491" spans="1:8">
+    <row r="491" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A491">
         <v>2.2000000000000002</v>
       </c>
@@ -13337,7 +13344,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="492" spans="1:8">
+    <row r="492" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A492">
         <v>4.5</v>
       </c>
@@ -13360,7 +13367,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="493" spans="1:8">
+    <row r="493" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A493">
         <v>4.2</v>
       </c>
@@ -13383,7 +13390,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="494" spans="1:8">
+    <row r="494" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A494">
         <v>5</v>
       </c>
@@ -13406,7 +13413,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="495" spans="1:8">
+    <row r="495" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A495" s="1">
         <v>27.69</v>
       </c>
@@ -13430,7 +13437,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="496" spans="1:8">
+    <row r="496" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A496">
         <v>70</v>
       </c>
@@ -13453,7 +13460,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="497" spans="1:8">
+    <row r="497" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A497" s="1">
         <v>2.2999999999999998</v>
       </c>
@@ -13477,7 +13484,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="498" spans="1:8">
+    <row r="498" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A498">
         <v>3.2</v>
       </c>
@@ -13500,7 +13507,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="499" spans="1:8">
+    <row r="499" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A499">
         <v>3.6</v>
       </c>
@@ -13523,7 +13530,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="500" spans="1:8">
+    <row r="500" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A500">
         <v>0.5</v>
       </c>
@@ -13546,7 +13553,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="501" spans="1:8">
+    <row r="501" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A501">
         <v>10</v>
       </c>
@@ -13569,7 +13576,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="502" spans="1:8">
+    <row r="502" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A502">
         <v>2</v>
       </c>
@@ -13592,7 +13599,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="503" spans="1:8">
+    <row r="503" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A503" s="1">
         <v>1.9</v>
       </c>
@@ -13616,7 +13623,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="504" spans="1:8">
+    <row r="504" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A504">
         <v>6.6</v>
       </c>
@@ -13639,7 +13646,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="505" spans="1:8">
+    <row r="505" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A505">
         <v>1.8</v>
       </c>
@@ -13662,7 +13669,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="506" spans="1:8">
+    <row r="506" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A506" s="1">
         <v>0.8</v>
       </c>
@@ -13686,7 +13693,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="507" spans="1:8">
+    <row r="507" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A507">
         <v>4.2</v>
       </c>
@@ -13709,7 +13716,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="508" spans="1:8">
+    <row r="508" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A508">
         <v>4</v>
       </c>
@@ -13732,7 +13739,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="509" spans="1:8">
+    <row r="509" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A509">
         <v>1.2</v>
       </c>
@@ -13755,7 +13762,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="510" spans="1:8">
+    <row r="510" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A510">
         <v>5</v>
       </c>
@@ -13778,7 +13785,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="511" spans="1:8">
+    <row r="511" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A511">
         <v>3.5</v>
       </c>
@@ -13801,7 +13808,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="512" spans="1:8">
+    <row r="512" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A512" s="1">
         <v>1.75</v>
       </c>
@@ -13825,7 +13832,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="513" spans="1:8">
+    <row r="513" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A513">
         <v>4.2</v>
       </c>
@@ -13848,7 +13855,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="514" spans="1:8">
+    <row r="514" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A514">
         <v>5.6</v>
       </c>
@@ -13871,7 +13878,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="515" spans="1:8">
+    <row r="515" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A515">
         <v>3.6</v>
       </c>
@@ -13894,7 +13901,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="516" spans="1:8">
+    <row r="516" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A516">
         <v>15.93</v>
       </c>
@@ -13917,7 +13924,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="517" spans="1:8">
+    <row r="517" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A517">
         <v>5.98</v>
       </c>
@@ -13940,7 +13947,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="518" spans="1:8">
+    <row r="518" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A518">
         <v>5</v>
       </c>
@@ -13963,7 +13970,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="519" spans="1:8">
+    <row r="519" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A519">
         <v>4.2</v>
       </c>
@@ -13986,7 +13993,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="520" spans="1:8">
+    <row r="520" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A520">
         <v>4.2</v>
       </c>
@@ -14009,7 +14016,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="521" spans="1:8">
+    <row r="521" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A521">
         <v>4</v>
       </c>
@@ -14032,7 +14039,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="522" spans="1:8">
+    <row r="522" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A522">
         <v>3</v>
       </c>
@@ -14055,7 +14062,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="523" spans="1:8">
+    <row r="523" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A523">
         <v>2</v>
       </c>
@@ -14078,7 +14085,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="524" spans="1:8">
+    <row r="524" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A524">
         <v>1</v>
       </c>
@@ -14101,7 +14108,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="525" spans="1:8">
+    <row r="525" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A525" s="1">
         <v>4.0999999999999996</v>
       </c>
@@ -14125,7 +14132,30 @@
         <v>250</v>
       </c>
     </row>
-    <row r="528" spans="1:8">
+    <row r="526" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A526">
+        <v>78.180000000000007</v>
+      </c>
+      <c r="B526" t="s">
+        <v>351</v>
+      </c>
+      <c r="C526" s="2">
+        <v>43396</v>
+      </c>
+      <c r="D526" t="s">
+        <v>520</v>
+      </c>
+      <c r="E526" t="s">
+        <v>238</v>
+      </c>
+      <c r="F526">
+        <v>5</v>
+      </c>
+      <c r="H526" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="528" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C528" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gamw thn Green Mani
</commit_message>
<xml_diff>
--- a/DataBase/costs.xlsx
+++ b/DataBase/costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2205" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2221" uniqueCount="541">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1628,6 +1628,15 @@
   </si>
   <si>
     <t>crepa σοκολάτα με μπανανα και μπικότο, μπάρα πρωτεΐνης</t>
+  </si>
+  <si>
+    <t>πατατάκια, monster και σοκολάτα CRANCH</t>
+  </si>
+  <si>
+    <t>axe αποσμυτικό και τσίχλες</t>
+  </si>
+  <si>
+    <t>καλτσόνε και κουλούρι θεσσαλονίκης</t>
   </si>
 </sst>
 </file>
@@ -1763,7 +1772,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:H549" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:H553" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="8">
     <tableColumn id="1" name="amount" headerRowDxfId="8" totalsRowDxfId="7"/>
     <tableColumn id="11" name="type" totalsRowDxfId="6"/>
@@ -2065,10 +2074,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L549"/>
+  <dimension ref="A1:L553"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A528" workbookViewId="0">
-      <selection activeCell="H550" sqref="H550"/>
+      <selection activeCell="A554" sqref="A554"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14745,6 +14754,98 @@
         <v>243</v>
       </c>
     </row>
+    <row r="550" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A550">
+        <v>4.8</v>
+      </c>
+      <c r="B550" t="s">
+        <v>217</v>
+      </c>
+      <c r="C550" s="7">
+        <v>43410</v>
+      </c>
+      <c r="D550" t="s">
+        <v>538</v>
+      </c>
+      <c r="E550" t="s">
+        <v>231</v>
+      </c>
+      <c r="F550">
+        <v>5</v>
+      </c>
+      <c r="H550" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="551" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A551">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="B551" t="s">
+        <v>335</v>
+      </c>
+      <c r="C551" s="7">
+        <v>43410</v>
+      </c>
+      <c r="D551" t="s">
+        <v>539</v>
+      </c>
+      <c r="E551" t="s">
+        <v>231</v>
+      </c>
+      <c r="F551">
+        <v>5</v>
+      </c>
+      <c r="H551" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="552" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A552">
+        <v>2.6</v>
+      </c>
+      <c r="B552" t="s">
+        <v>217</v>
+      </c>
+      <c r="C552" s="7">
+        <v>43410</v>
+      </c>
+      <c r="D552" t="s">
+        <v>540</v>
+      </c>
+      <c r="E552" t="s">
+        <v>231</v>
+      </c>
+      <c r="F552">
+        <v>5</v>
+      </c>
+      <c r="H552" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="553" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A553">
+        <v>3.7</v>
+      </c>
+      <c r="B553" t="s">
+        <v>217</v>
+      </c>
+      <c r="C553" s="2">
+        <v>43410</v>
+      </c>
+      <c r="D553" t="s">
+        <v>117</v>
+      </c>
+      <c r="E553" t="s">
+        <v>231</v>
+      </c>
+      <c r="F553">
+        <v>3</v>
+      </c>
+      <c r="H553" t="s">
+        <v>243</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Start to create FiltersByDate
</commit_message>
<xml_diff>
--- a/DataBase/costs.xlsx
+++ b/DataBase/costs.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="costs" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2221" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2229" uniqueCount="543">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1637,6 +1637,12 @@
   </si>
   <si>
     <t>καλτσόνε και κουλούρι θεσσαλονίκης</t>
+  </si>
+  <si>
+    <t>3 παντελόνια</t>
+  </si>
+  <si>
+    <t>pancake και smooothie με banana, yogurt and chocolate</t>
   </si>
 </sst>
 </file>
@@ -1772,7 +1778,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:H553" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:H555" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="8">
     <tableColumn id="1" name="amount" headerRowDxfId="8" totalsRowDxfId="7"/>
     <tableColumn id="11" name="type" totalsRowDxfId="6"/>
@@ -2074,10 +2080,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L553"/>
+  <dimension ref="A1:L555"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A528" workbookViewId="0">
-      <selection activeCell="A554" sqref="A554"/>
+      <selection activeCell="B556" sqref="B556"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14846,6 +14852,52 @@
         <v>243</v>
       </c>
     </row>
+    <row r="554" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A554">
+        <v>120</v>
+      </c>
+      <c r="B554" t="s">
+        <v>217</v>
+      </c>
+      <c r="C554" s="2">
+        <v>43410</v>
+      </c>
+      <c r="D554" t="s">
+        <v>541</v>
+      </c>
+      <c r="E554" t="s">
+        <v>231</v>
+      </c>
+      <c r="F554">
+        <v>5</v>
+      </c>
+      <c r="H554" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="555" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A555">
+        <v>6.8</v>
+      </c>
+      <c r="B555" t="s">
+        <v>217</v>
+      </c>
+      <c r="C555" s="2">
+        <v>43411</v>
+      </c>
+      <c r="D555" t="s">
+        <v>542</v>
+      </c>
+      <c r="E555" t="s">
+        <v>231</v>
+      </c>
+      <c r="F555">
+        <v>5</v>
+      </c>
+      <c r="H555" t="s">
+        <v>243</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update database with launch
</commit_message>
<xml_diff>
--- a/DataBase/costs.xlsx
+++ b/DataBase/costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2513" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2517" uniqueCount="610">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1841,6 +1841,9 @@
   </si>
   <si>
     <t>μπουγάτσα με σοκολάτα και μπουγάτσα με τυρί</t>
+  </si>
+  <si>
+    <t>πέννες φούρνου και 10 σκορδόψωμα</t>
   </si>
 </sst>
 </file>
@@ -1984,7 +1987,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:I626" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:I627" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="9">
     <tableColumn id="1" name="amount" headerRowDxfId="9" totalsRowDxfId="8"/>
     <tableColumn id="11" name="type" totalsRowDxfId="7"/>
@@ -2287,10 +2290,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L626"/>
+  <dimension ref="A1:L627"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A618" workbookViewId="0">
-      <selection activeCell="F630" sqref="F630"/>
+      <selection activeCell="A628" sqref="A628"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16740,6 +16743,29 @@
         <v>243</v>
       </c>
     </row>
+    <row r="627" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A627">
+        <v>9</v>
+      </c>
+      <c r="B627" t="s">
+        <v>217</v>
+      </c>
+      <c r="C627" s="2">
+        <v>43441</v>
+      </c>
+      <c r="D627" t="s">
+        <v>609</v>
+      </c>
+      <c r="E627" t="s">
+        <v>231</v>
+      </c>
+      <c r="F627">
+        <v>5</v>
+      </c>
+      <c r="H627" t="s">
+        <v>243</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update windows and pay for a key on ebay
</commit_message>
<xml_diff>
--- a/DataBase/costs.xlsx
+++ b/DataBase/costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3697" uniqueCount="714">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3702" uniqueCount="715">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -2156,6 +2156,9 @@
   </si>
   <si>
     <t>εισητήρια για Θεσσαλονίκη</t>
+  </si>
+  <si>
+    <t>κλειδί για αναβάθμιση σε windows Pro</t>
   </si>
 </sst>
 </file>
@@ -2307,7 +2310,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:J737" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:J738" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="10">
     <tableColumn id="1" name="amount" headerRowDxfId="10" totalsRowDxfId="9"/>
     <tableColumn id="11" name="type" totalsRowDxfId="8"/>
@@ -2609,10 +2612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L737"/>
+  <dimension ref="A1:L738"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A715" workbookViewId="0">
-      <selection activeCell="A738" sqref="A738"/>
+    <sheetView tabSelected="1" topLeftCell="B717" workbookViewId="0">
+      <selection activeCell="H739" sqref="H739"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24098,6 +24101,36 @@
         <v>660</v>
       </c>
     </row>
+    <row r="738" spans="1:10">
+      <c r="A738" s="1">
+        <v>6.03</v>
+      </c>
+      <c r="B738" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C738" s="7">
+        <v>43494</v>
+      </c>
+      <c r="D738" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="E738" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F738" s="1">
+        <v>4</v>
+      </c>
+      <c r="G738" s="1"/>
+      <c r="H738" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="I738" s="1">
+        <v>736</v>
+      </c>
+      <c r="J738" s="1" t="s">
+        <v>660</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update cost for my Birthday
</commit_message>
<xml_diff>
--- a/DataBase/costs.xlsx
+++ b/DataBase/costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3726" uniqueCount="718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3731" uniqueCount="719">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -2168,6 +2168,9 @@
   </si>
   <si>
     <t>Ελληνική ομελέτα στο underdog</t>
+  </si>
+  <si>
+    <t>1kg μπακλαβαδάκια για κέρασμα από τον Βενέτη</t>
   </si>
 </sst>
 </file>
@@ -2319,7 +2322,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:J743" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:J744" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="10">
     <tableColumn id="1" name="amount" headerRowDxfId="10" totalsRowDxfId="9"/>
     <tableColumn id="11" name="type" totalsRowDxfId="8"/>
@@ -2621,10 +2624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L743"/>
+  <dimension ref="A1:L744"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B70" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+    <sheetView tabSelected="1" topLeftCell="A729" workbookViewId="0">
+      <selection activeCell="A745" sqref="A745"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24290,6 +24293,36 @@
         <v>660</v>
       </c>
     </row>
+    <row r="744" spans="1:10">
+      <c r="A744" s="1">
+        <v>16.09</v>
+      </c>
+      <c r="B744" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C744" s="7">
+        <v>43501</v>
+      </c>
+      <c r="D744" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="E744" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F744" s="1">
+        <v>5</v>
+      </c>
+      <c r="G744" s="1"/>
+      <c r="H744" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="I744" s="1">
+        <v>742</v>
+      </c>
+      <c r="J744" s="1" t="s">
+        <v>651</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
H agilara paei agglia
</commit_message>
<xml_diff>
--- a/DataBase/costs.xlsx
+++ b/DataBase/costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3786" uniqueCount="730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3801" uniqueCount="733">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -2204,6 +2204,15 @@
   </si>
   <si>
     <t>φαγητό στον Αδάμ</t>
+  </si>
+  <si>
+    <t>"γρήγορη" κάρτα μνήμης για την φωτογραφική</t>
+  </si>
+  <si>
+    <t>μιλήτη στην Arch με γεωργία ρουβά και στέλιο</t>
+  </si>
+  <si>
+    <t>σουβλάκι με μπιφτέκι λαχανικών και πατάτες τηγανιτές</t>
   </si>
 </sst>
 </file>
@@ -2331,15 +2340,15 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2355,9 +2364,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:J755" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:J758" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="10">
-    <tableColumn id="1" name="amount" headerRowDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="1" name="amount" headerRowDxfId="9" totalsRowDxfId="10"/>
     <tableColumn id="11" name="type" totalsRowDxfId="8"/>
     <tableColumn id="2" name="date" totalsRowDxfId="7"/>
     <tableColumn id="4" name="description" totalsRowDxfId="6"/>
@@ -2657,10 +2666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L755"/>
+  <dimension ref="A1:L758"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E736" workbookViewId="0">
-      <selection activeCell="J753" sqref="J753:J755"/>
+    <sheetView tabSelected="1" topLeftCell="C737" workbookViewId="0">
+      <selection activeCell="J755" sqref="J755:J758"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24685,6 +24694,94 @@
         <v>645</v>
       </c>
     </row>
+    <row r="756" spans="1:10">
+      <c r="A756" s="1">
+        <v>24.9</v>
+      </c>
+      <c r="B756" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C756" s="7">
+        <v>43507</v>
+      </c>
+      <c r="D756" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="E756" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F756" s="1">
+        <v>5</v>
+      </c>
+      <c r="G756" s="1"/>
+      <c r="H756" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="I756" s="1">
+        <v>754</v>
+      </c>
+      <c r="J756" s="1" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="757" spans="1:10">
+      <c r="A757">
+        <v>5.5</v>
+      </c>
+      <c r="B757" t="s">
+        <v>211</v>
+      </c>
+      <c r="C757" s="7">
+        <v>43507</v>
+      </c>
+      <c r="D757" t="s">
+        <v>731</v>
+      </c>
+      <c r="E757" t="s">
+        <v>226</v>
+      </c>
+      <c r="F757">
+        <v>5</v>
+      </c>
+      <c r="H757" t="s">
+        <v>228</v>
+      </c>
+      <c r="I757" s="1">
+        <v>755</v>
+      </c>
+      <c r="J757" s="1" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="758" spans="1:10">
+      <c r="A758">
+        <v>4.2</v>
+      </c>
+      <c r="B758" t="s">
+        <v>211</v>
+      </c>
+      <c r="C758" s="7">
+        <v>43507</v>
+      </c>
+      <c r="D758" t="s">
+        <v>732</v>
+      </c>
+      <c r="E758" t="s">
+        <v>226</v>
+      </c>
+      <c r="F758">
+        <v>5</v>
+      </c>
+      <c r="H758" t="s">
+        <v>228</v>
+      </c>
+      <c r="I758" s="1">
+        <v>756</v>
+      </c>
+      <c r="J758" s="1" t="s">
+        <v>645</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Trying to hack those nukes...just kidding
</commit_message>
<xml_diff>
--- a/DataBase/costs.xlsx
+++ b/DataBase/costs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="18975" windowHeight="11760"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="costs" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3801" uniqueCount="733">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3805" uniqueCount="734">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -2213,6 +2213,9 @@
   </si>
   <si>
     <t>σουβλάκι με μπιφτέκι λαχανικών και πατάτες τηγανιτές</t>
+  </si>
+  <si>
+    <t>Wireless adapter for hacking</t>
   </si>
 </sst>
 </file>
@@ -2220,8 +2223,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="6" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -2257,9 +2260,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
@@ -2340,15 +2343,15 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2364,9 +2367,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:J758" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:J759" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="10">
-    <tableColumn id="1" name="amount" headerRowDxfId="9" totalsRowDxfId="10"/>
+    <tableColumn id="1" name="amount" headerRowDxfId="10" totalsRowDxfId="9"/>
     <tableColumn id="11" name="type" totalsRowDxfId="8"/>
     <tableColumn id="2" name="date" totalsRowDxfId="7"/>
     <tableColumn id="4" name="description" totalsRowDxfId="6"/>
@@ -2666,10 +2669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L758"/>
+  <dimension ref="A1:L759"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C737" workbookViewId="0">
-      <selection activeCell="J755" sqref="J755:J758"/>
+    <sheetView tabSelected="1" topLeftCell="A739" workbookViewId="0">
+      <selection activeCell="I759" sqref="I759"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24782,6 +24785,30 @@
         <v>645</v>
       </c>
     </row>
+    <row r="759" spans="1:10">
+      <c r="A759" s="1">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="B759" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C759" s="1"/>
+      <c r="D759" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="E759" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F759" s="1">
+        <v>5</v>
+      </c>
+      <c r="G759" s="1"/>
+      <c r="H759" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="I759" s="1"/>
+      <c r="J759" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
1, 2 to ksereiw sagapw
</commit_message>
<xml_diff>
--- a/DataBase/costs.xlsx
+++ b/DataBase/costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3851" uniqueCount="741">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3866" uniqueCount="744">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -2237,6 +2237,15 @@
   </si>
   <si>
     <t>rise in street wok</t>
+  </si>
+  <si>
+    <t>κουλούρι και φυσικό από το κυλικείο της σχολής</t>
+  </si>
+  <si>
+    <t>monster doctor</t>
+  </si>
+  <si>
+    <t>προφυλακτικά</t>
   </si>
 </sst>
 </file>
@@ -2388,7 +2397,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:J768" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:J771" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="10">
     <tableColumn id="1" name="amount" headerRowDxfId="10" totalsRowDxfId="9"/>
     <tableColumn id="11" name="type" totalsRowDxfId="8"/>
@@ -2690,10 +2699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L769"/>
+  <dimension ref="A1:L771"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A268" workbookViewId="0">
-      <selection activeCell="D280" sqref="D280"/>
+    <sheetView tabSelected="1" topLeftCell="B757" workbookViewId="0">
+      <selection activeCell="E774" sqref="E774"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -25104,8 +25113,95 @@
         <v>639</v>
       </c>
     </row>
-    <row r="769" spans="9:9">
-      <c r="I769" s="1"/>
+    <row r="769" spans="1:10">
+      <c r="A769" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="B769" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C769" s="7">
+        <v>43515</v>
+      </c>
+      <c r="D769" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="E769" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F769" s="1">
+        <v>5</v>
+      </c>
+      <c r="G769" s="1"/>
+      <c r="H769" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="I769" s="1">
+        <v>767</v>
+      </c>
+      <c r="J769" s="1" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="770" spans="1:10">
+      <c r="A770" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B770" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C770" s="7">
+        <v>43515</v>
+      </c>
+      <c r="D770" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="E770" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F770" s="1">
+        <v>5</v>
+      </c>
+      <c r="G770" s="1"/>
+      <c r="H770" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="I770" s="1">
+        <v>768</v>
+      </c>
+      <c r="J770" s="1" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="771" spans="1:10">
+      <c r="A771" s="1">
+        <v>6.4</v>
+      </c>
+      <c r="B771" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C771" s="7">
+        <v>43515</v>
+      </c>
+      <c r="D771" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="E771" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F771" s="1">
+        <v>5</v>
+      </c>
+      <c r="G771" s="1"/>
+      <c r="H771" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I771" s="1">
+        <v>769</v>
+      </c>
+      <c r="J771" s="1" t="s">
+        <v>641</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>